<commit_message>
age groups for data definitions
</commit_message>
<xml_diff>
--- a/_Code/dhs_variable_definitions.xlsx
+++ b/_Code/dhs_variable_definitions.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnpainter/Dropbox/_Malaria/Projects/DHS/_Code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bzp3\dropbox\_Malaria\Projects\DHS\_Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="84" yWindow="456" windowWidth="25524" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="definitions" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="275">
   <si>
     <t>Variable</t>
   </si>
@@ -839,12 +839,27 @@
   </si>
   <si>
     <t>Country code and phase</t>
+  </si>
+  <si>
+    <t>addNA( cut( hml16, breaks= c(0,5,15,25,35,45, Inf) )  )</t>
+  </si>
+  <si>
+    <t>Age groups</t>
+  </si>
+  <si>
+    <t>age.grp</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dummy variable for counting </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -1172,24 +1187,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J89"/>
+  <dimension ref="A1:J92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="30" customWidth="1"/>
-    <col min="2" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="15.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.796875" customWidth="1"/>
     <col min="4" max="4" width="55.5" customWidth="1"/>
-    <col min="5" max="5" width="58.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="58.69921875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
-    <col min="9" max="9" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1221,7 +1236,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>142</v>
       </c>
@@ -1244,29 +1259,26 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>273</v>
+      </c>
+      <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>274</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>60</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>145</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
@@ -1275,15 +1287,18 @@
         <v>60</v>
       </c>
       <c r="D5" t="s">
-        <v>146</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
@@ -1292,18 +1307,15 @@
         <v>60</v>
       </c>
       <c r="D6" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E6" t="s">
-        <v>150</v>
-      </c>
-      <c r="J6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>148</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
@@ -1312,38 +1324,38 @@
         <v>60</v>
       </c>
       <c r="D7" t="s">
+        <v>149</v>
+      </c>
+      <c r="E7" t="s">
+        <v>150</v>
+      </c>
+      <c r="J7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>4</v>
       </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>151</v>
-      </c>
-      <c r="B10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" t="s">
-        <v>60</v>
-      </c>
-      <c r="D10" t="s">
-        <v>152</v>
-      </c>
-      <c r="E10" t="s">
-        <v>153</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>154</v>
       </c>
       <c r="B11" t="s">
         <v>7</v>
@@ -1352,18 +1364,18 @@
         <v>60</v>
       </c>
       <c r="D11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="E11" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="B12" t="s">
         <v>7</v>
@@ -1375,15 +1387,15 @@
         <v>155</v>
       </c>
       <c r="E12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>157</v>
       </c>
       <c r="B13" t="s">
         <v>7</v>
@@ -1392,98 +1404,75 @@
         <v>60</v>
       </c>
       <c r="D13" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13" t="s">
+        <v>158</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>60</v>
+      </c>
+      <c r="D14" t="s">
         <v>159</v>
       </c>
-      <c r="E13" t="s">
+      <c r="E14" t="s">
         <v>62</v>
       </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="G14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>19</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>58</v>
-      </c>
-      <c r="C16" t="s">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>160</v>
-      </c>
-      <c r="E16" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>161</v>
       </c>
       <c r="C17" t="s">
         <v>60</v>
       </c>
       <c r="D17" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E17" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="G17">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>272</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
         <v>60</v>
       </c>
       <c r="D18" t="s">
-        <v>164</v>
+        <v>271</v>
       </c>
       <c r="E18" t="s">
-        <v>165</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>166</v>
-      </c>
-      <c r="B19" t="s">
-        <v>161</v>
-      </c>
-      <c r="C19" t="s">
-        <v>60</v>
-      </c>
-      <c r="D19" t="s">
-        <v>167</v>
-      </c>
-      <c r="E19" t="s">
-        <v>168</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>169</v>
+        <v>12</v>
       </c>
       <c r="B20" t="s">
         <v>161</v>
@@ -1492,78 +1481,78 @@
         <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="E20" t="s">
-        <v>171</v>
+        <v>13</v>
       </c>
       <c r="G20">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" t="s">
+        <v>161</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>164</v>
+      </c>
+      <c r="E21" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="B22" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C22" t="s">
         <v>60</v>
       </c>
       <c r="D22" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="E22" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="G22">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="B23" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
         <v>60</v>
       </c>
       <c r="D23" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="E23" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="G23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>178</v>
-      </c>
-      <c r="B24" t="s">
-        <v>58</v>
-      </c>
-      <c r="C24" t="s">
-        <v>60</v>
-      </c>
-      <c r="D24" t="s">
-        <v>179</v>
-      </c>
-      <c r="E24" t="s">
-        <v>180</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B25" t="s">
         <v>58</v>
@@ -1572,87 +1561,78 @@
         <v>60</v>
       </c>
       <c r="D25" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="E25" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="G25">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>175</v>
+      </c>
+      <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>176</v>
+      </c>
+      <c r="E26" t="s">
+        <v>177</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>57</v>
+        <v>178</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
       </c>
       <c r="C27" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D27" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E27" t="s">
-        <v>22</v>
+        <v>180</v>
       </c>
       <c r="G27">
-        <v>1</v>
-      </c>
-      <c r="H27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>42</v>
+        <v>181</v>
       </c>
       <c r="B28" t="s">
         <v>58</v>
       </c>
       <c r="C28" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="E28" t="s">
-        <v>23</v>
+        <v>183</v>
       </c>
       <c r="G28">
-        <v>1</v>
-      </c>
-      <c r="H28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>186</v>
-      </c>
-      <c r="B29" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" t="s">
-        <v>59</v>
-      </c>
-      <c r="D29" t="s">
-        <v>187</v>
-      </c>
-      <c r="E29" t="s">
-        <v>188</v>
-      </c>
-      <c r="G29">
-        <v>1</v>
-      </c>
-      <c r="H29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
@@ -1661,10 +1641,10 @@
         <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E30" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G30">
         <v>1</v>
@@ -1673,21 +1653,44 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" t="s">
+        <v>59</v>
+      </c>
+      <c r="D31" t="s">
+        <v>185</v>
+      </c>
+      <c r="E31" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C32" t="s">
         <v>59</v>
       </c>
       <c r="D32" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="E32" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="G32">
         <v>1</v>
@@ -1696,55 +1699,32 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
         <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="E33" t="s">
-        <v>194</v>
+        <v>24</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>148</v>
-      </c>
-      <c r="B34" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" t="s">
-        <v>59</v>
-      </c>
-      <c r="D34" t="s">
-        <v>191</v>
-      </c>
-      <c r="E34" t="s">
-        <v>195</v>
-      </c>
-      <c r="G34">
-        <v>1</v>
-      </c>
-      <c r="H34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="B35" t="s">
         <v>7</v>
@@ -1753,21 +1733,44 @@
         <v>59</v>
       </c>
       <c r="D35" t="s">
+        <v>191</v>
+      </c>
+      <c r="E35" t="s">
+        <v>192</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>6</v>
+      </c>
+      <c r="B36" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" t="s">
         <v>193</v>
       </c>
-      <c r="E35" t="s">
-        <v>196</v>
-      </c>
-      <c r="G35">
-        <v>1</v>
-      </c>
-      <c r="H35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E36" t="s">
+        <v>194</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>43</v>
+        <v>148</v>
       </c>
       <c r="B37" t="s">
         <v>7</v>
@@ -1776,10 +1779,10 @@
         <v>59</v>
       </c>
       <c r="D37" t="s">
-        <v>197</v>
+        <v>191</v>
       </c>
       <c r="E37" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G37">
         <v>1</v>
@@ -1788,9 +1791,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>11</v>
+        <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>7</v>
@@ -1799,10 +1802,10 @@
         <v>59</v>
       </c>
       <c r="D38" t="s">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="E38" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G38">
         <v>1</v>
@@ -1811,32 +1814,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>201</v>
-      </c>
-      <c r="B39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" t="s">
-        <v>197</v>
-      </c>
-      <c r="E39" t="s">
-        <v>202</v>
-      </c>
-      <c r="G39">
-        <v>1</v>
-      </c>
-      <c r="H39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>203</v>
+        <v>43</v>
       </c>
       <c r="B40" t="s">
         <v>7</v>
@@ -1845,21 +1825,44 @@
         <v>59</v>
       </c>
       <c r="D40" t="s">
+        <v>197</v>
+      </c>
+      <c r="E40" t="s">
+        <v>198</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>11</v>
+      </c>
+      <c r="B41" t="s">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" t="s">
         <v>199</v>
       </c>
-      <c r="E40" t="s">
-        <v>204</v>
-      </c>
-      <c r="G40">
-        <v>1</v>
-      </c>
-      <c r="H40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E41" t="s">
+        <v>200</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>44</v>
+        <v>201</v>
       </c>
       <c r="B42" t="s">
         <v>7</v>
@@ -1868,10 +1871,10 @@
         <v>59</v>
       </c>
       <c r="D42" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="E42" t="s">
-        <v>25</v>
+        <v>202</v>
       </c>
       <c r="G42">
         <v>1</v>
@@ -1880,9 +1883,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>15</v>
+        <v>203</v>
       </c>
       <c r="B43" t="s">
         <v>7</v>
@@ -1891,10 +1894,10 @@
         <v>59</v>
       </c>
       <c r="D43" t="s">
-        <v>206</v>
+        <v>199</v>
       </c>
       <c r="E43" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G43">
         <v>1</v>
@@ -1903,29 +1906,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>208</v>
-      </c>
-      <c r="B44" t="s">
-        <v>7</v>
-      </c>
-      <c r="C44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" t="s">
-        <v>205</v>
-      </c>
-      <c r="E44" t="s">
-        <v>209</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>210</v>
+        <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>7</v>
@@ -1934,18 +1917,44 @@
         <v>59</v>
       </c>
       <c r="D45" t="s">
+        <v>205</v>
+      </c>
+      <c r="E45" t="s">
+        <v>25</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" t="s">
         <v>206</v>
       </c>
-      <c r="E45" t="s">
-        <v>211</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E46" t="s">
+        <v>207</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>151</v>
+        <v>208</v>
       </c>
       <c r="B47" t="s">
         <v>7</v>
@@ -1954,44 +1963,38 @@
         <v>59</v>
       </c>
       <c r="D47" t="s">
-        <v>212</v>
+        <v>205</v>
       </c>
       <c r="E47" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="G47">
-        <v>1</v>
-      </c>
-      <c r="H47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
-        <v>154</v>
-      </c>
-      <c r="B49" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>210</v>
+      </c>
+      <c r="B48" t="s">
         <v>7</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C48" t="s">
         <v>59</v>
       </c>
-      <c r="D49" t="s">
-        <v>155</v>
-      </c>
-      <c r="E49" t="s">
-        <v>214</v>
-      </c>
-      <c r="G49">
-        <v>1</v>
-      </c>
-      <c r="H49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="D48" t="s">
+        <v>206</v>
+      </c>
+      <c r="E48" t="s">
+        <v>211</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="B50" t="s">
         <v>7</v>
@@ -2000,10 +2003,10 @@
         <v>59</v>
       </c>
       <c r="D50" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="E50" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="G50">
         <v>1</v>
@@ -2012,22 +2015,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="26" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>154</v>
       </c>
       <c r="B52" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
         <v>59</v>
       </c>
       <c r="D52" t="s">
-        <v>37</v>
+        <v>155</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>214</v>
       </c>
       <c r="G52">
         <v>1</v>
@@ -2036,21 +2038,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>157</v>
       </c>
       <c r="B53" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="C53" t="s">
         <v>59</v>
       </c>
       <c r="D53" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
       <c r="E53" t="s">
-        <v>35</v>
+        <v>215</v>
       </c>
       <c r="G53">
         <v>1</v>
@@ -2059,32 +2061,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>163</v>
-      </c>
-      <c r="B54" t="s">
-        <v>161</v>
-      </c>
-      <c r="C54" t="s">
-        <v>59</v>
-      </c>
-      <c r="D54" t="s">
-        <v>216</v>
-      </c>
-      <c r="E54" t="s">
-        <v>217</v>
-      </c>
-      <c r="G54">
-        <v>1</v>
-      </c>
-      <c r="H54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:10" ht="25.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B55" t="s">
         <v>161</v>
@@ -2093,24 +2073,21 @@
         <v>59</v>
       </c>
       <c r="D55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E55" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="G55">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H55">
-        <v>0</v>
-      </c>
-      <c r="J55" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>218</v>
+        <v>46</v>
       </c>
       <c r="B56" t="s">
         <v>161</v>
@@ -2119,24 +2096,21 @@
         <v>59</v>
       </c>
       <c r="D56" t="s">
-        <v>219</v>
+        <v>36</v>
       </c>
       <c r="E56" t="s">
-        <v>220</v>
+        <v>35</v>
       </c>
       <c r="G56">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H56">
-        <v>0</v>
-      </c>
-      <c r="J56" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>48</v>
+        <v>163</v>
       </c>
       <c r="B57" t="s">
         <v>161</v>
@@ -2145,24 +2119,21 @@
         <v>59</v>
       </c>
       <c r="D57" t="s">
-        <v>39</v>
+        <v>216</v>
       </c>
       <c r="E57" t="s">
-        <v>27</v>
+        <v>217</v>
       </c>
       <c r="G57">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57">
-        <v>0</v>
-      </c>
-      <c r="J57" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>47</v>
       </c>
       <c r="B58" t="s">
         <v>161</v>
@@ -2171,81 +2142,99 @@
         <v>59</v>
       </c>
       <c r="D58" t="s">
+        <v>40</v>
+      </c>
+      <c r="E58" t="s">
+        <v>26</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="J58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>218</v>
+      </c>
+      <c r="B59" t="s">
+        <v>161</v>
+      </c>
+      <c r="C59" t="s">
+        <v>59</v>
+      </c>
+      <c r="D59" t="s">
+        <v>219</v>
+      </c>
+      <c r="E59" t="s">
+        <v>220</v>
+      </c>
+      <c r="G59">
+        <v>0</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+      <c r="J59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" t="s">
+        <v>161</v>
+      </c>
+      <c r="C60" t="s">
+        <v>59</v>
+      </c>
+      <c r="D60" t="s">
+        <v>39</v>
+      </c>
+      <c r="E60" t="s">
+        <v>27</v>
+      </c>
+      <c r="G60">
+        <v>0</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+      <c r="J60" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>166</v>
+      </c>
+      <c r="B61" t="s">
+        <v>161</v>
+      </c>
+      <c r="C61" t="s">
+        <v>59</v>
+      </c>
+      <c r="D61" t="s">
         <v>221</v>
       </c>
-      <c r="E58" t="s">
+      <c r="E61" t="s">
         <v>222</v>
       </c>
-      <c r="G58">
-        <v>0</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63" t="s">
+      <c r="G61">
+        <v>0</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
         <v>49</v>
-      </c>
-      <c r="B63" t="s">
-        <v>58</v>
-      </c>
-      <c r="C63" t="s">
-        <v>59</v>
-      </c>
-      <c r="E63" t="s">
-        <v>29</v>
-      </c>
-      <c r="G63">
-        <v>0</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>50</v>
-      </c>
-      <c r="B64" t="s">
-        <v>58</v>
-      </c>
-      <c r="C64" t="s">
-        <v>59</v>
-      </c>
-      <c r="E64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G64">
-        <v>0</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A65" t="s">
-        <v>223</v>
-      </c>
-      <c r="B65" t="s">
-        <v>58</v>
-      </c>
-      <c r="C65" t="s">
-        <v>59</v>
-      </c>
-      <c r="E65" t="s">
-        <v>224</v>
-      </c>
-      <c r="G65">
-        <v>0</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>225</v>
       </c>
       <c r="B66" t="s">
         <v>58</v>
@@ -2254,18 +2243,18 @@
         <v>59</v>
       </c>
       <c r="E66" t="s">
-        <v>226</v>
+        <v>29</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>227</v>
+        <v>50</v>
       </c>
       <c r="B67" t="s">
         <v>58</v>
@@ -2273,22 +2262,19 @@
       <c r="C67" t="s">
         <v>59</v>
       </c>
-      <c r="D67" t="s">
-        <v>228</v>
-      </c>
       <c r="E67" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>230</v>
+        <v>223</v>
       </c>
       <c r="B68" t="s">
         <v>58</v>
@@ -2296,31 +2282,51 @@
       <c r="C68" t="s">
         <v>59</v>
       </c>
-      <c r="D68" t="s">
-        <v>231</v>
-      </c>
       <c r="E68" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>225</v>
+      </c>
+      <c r="B69" t="s">
+        <v>58</v>
+      </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
+      <c r="E69" t="s">
+        <v>226</v>
+      </c>
+      <c r="G69">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>41</v>
+        <v>227</v>
       </c>
       <c r="B70" t="s">
         <v>58</v>
       </c>
       <c r="C70" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="D70" t="s">
+        <v>228</v>
       </c>
       <c r="E70" t="s">
-        <v>30</v>
+        <v>229</v>
       </c>
       <c r="G70">
         <v>1</v>
@@ -2329,87 +2335,52 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A72" t="s">
-        <v>51</v>
-      </c>
-      <c r="B72" t="s">
-        <v>7</v>
-      </c>
-      <c r="C72" t="s">
-        <v>61</v>
-      </c>
-      <c r="D72" t="s">
-        <v>233</v>
-      </c>
-      <c r="E72" t="s">
-        <v>234</v>
-      </c>
-      <c r="G72">
-        <v>1</v>
-      </c>
-      <c r="H72">
-        <v>2</v>
-      </c>
-      <c r="I72" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>230</v>
+      </c>
+      <c r="B71" t="s">
+        <v>58</v>
+      </c>
+      <c r="C71" t="s">
+        <v>59</v>
+      </c>
+      <c r="D71" t="s">
+        <v>231</v>
+      </c>
+      <c r="E71" t="s">
+        <v>232</v>
+      </c>
+      <c r="G71">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>236</v>
+        <v>41</v>
       </c>
       <c r="B73" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
       <c r="C73" t="s">
         <v>61</v>
       </c>
-      <c r="D73" t="s">
-        <v>237</v>
-      </c>
       <c r="E73" t="s">
-        <v>238</v>
+        <v>30</v>
       </c>
       <c r="G73">
         <v>1</v>
       </c>
       <c r="H73">
-        <v>2</v>
-      </c>
-      <c r="I73" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>52</v>
-      </c>
-      <c r="B74" t="s">
-        <v>7</v>
-      </c>
-      <c r="C74" t="s">
-        <v>61</v>
-      </c>
-      <c r="D74" t="s">
-        <v>239</v>
-      </c>
-      <c r="E74" t="s">
-        <v>31</v>
-      </c>
-      <c r="G74">
-        <v>1</v>
-      </c>
-      <c r="H74">
-        <v>2</v>
-      </c>
-      <c r="I74" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>240</v>
+        <v>51</v>
       </c>
       <c r="B75" t="s">
         <v>7</v>
@@ -2418,10 +2389,10 @@
         <v>61</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E75" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="G75">
         <v>1</v>
@@ -2433,9 +2404,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>53</v>
+        <v>236</v>
       </c>
       <c r="B76" t="s">
         <v>7</v>
@@ -2444,10 +2415,10 @@
         <v>61</v>
       </c>
       <c r="D76" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="E76" t="s">
-        <v>32</v>
+        <v>238</v>
       </c>
       <c r="G76">
         <v>1</v>
@@ -2459,9 +2430,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>244</v>
+        <v>52</v>
       </c>
       <c r="B77" t="s">
         <v>7</v>
@@ -2470,10 +2441,10 @@
         <v>61</v>
       </c>
       <c r="D77" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="E77" t="s">
-        <v>246</v>
+        <v>31</v>
       </c>
       <c r="G77">
         <v>1</v>
@@ -2485,9 +2456,35 @@
         <v>235</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>240</v>
+      </c>
+      <c r="B78" t="s">
+        <v>7</v>
+      </c>
+      <c r="C78" t="s">
+        <v>61</v>
+      </c>
+      <c r="D78" t="s">
+        <v>241</v>
+      </c>
+      <c r="E78" t="s">
+        <v>242</v>
+      </c>
+      <c r="G78">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>247</v>
+        <v>53</v>
       </c>
       <c r="B79" t="s">
         <v>7</v>
@@ -2496,10 +2493,10 @@
         <v>61</v>
       </c>
       <c r="D79" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="E79" t="s">
-        <v>249</v>
+        <v>32</v>
       </c>
       <c r="G79">
         <v>1</v>
@@ -2511,9 +2508,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B80" t="s">
         <v>7</v>
@@ -2522,10 +2519,10 @@
         <v>61</v>
       </c>
       <c r="D80" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="E80" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="G80">
         <v>1</v>
@@ -2537,21 +2534,21 @@
         <v>235</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>54</v>
+        <v>247</v>
       </c>
       <c r="B82" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="C82" t="s">
         <v>61</v>
       </c>
       <c r="D82" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="E82" t="s">
-        <v>33</v>
+        <v>249</v>
       </c>
       <c r="G82">
         <v>1</v>
@@ -2563,21 +2560,21 @@
         <v>235</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>54</v>
+        <v>250</v>
       </c>
       <c r="B83" t="s">
-        <v>161</v>
+        <v>7</v>
       </c>
       <c r="C83" t="s">
         <v>61</v>
       </c>
       <c r="D83" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E83" t="s">
-        <v>33</v>
+        <v>252</v>
       </c>
       <c r="G83">
         <v>1</v>
@@ -2589,35 +2586,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A84" t="s">
-        <v>55</v>
-      </c>
-      <c r="B84" t="s">
-        <v>161</v>
-      </c>
-      <c r="C84" t="s">
-        <v>61</v>
-      </c>
-      <c r="D84" t="s">
-        <v>254</v>
-      </c>
-      <c r="E84" t="s">
-        <v>34</v>
-      </c>
-      <c r="G84">
-        <v>1</v>
-      </c>
-      <c r="H84">
-        <v>2</v>
-      </c>
-      <c r="I84" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>255</v>
+        <v>54</v>
       </c>
       <c r="B85" t="s">
         <v>161</v>
@@ -2626,10 +2597,10 @@
         <v>61</v>
       </c>
       <c r="D85" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E85" t="s">
-        <v>256</v>
+        <v>33</v>
       </c>
       <c r="G85">
         <v>1</v>
@@ -2641,9 +2612,9 @@
         <v>235</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>257</v>
+        <v>54</v>
       </c>
       <c r="B86" t="s">
         <v>161</v>
@@ -2652,10 +2623,10 @@
         <v>61</v>
       </c>
       <c r="D86" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="E86" t="s">
-        <v>259</v>
+        <v>33</v>
       </c>
       <c r="G86">
         <v>1</v>
@@ -2667,21 +2638,47 @@
         <v>235</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>55</v>
+      </c>
+      <c r="B87" t="s">
+        <v>161</v>
+      </c>
+      <c r="C87" t="s">
+        <v>61</v>
+      </c>
+      <c r="D87" t="s">
+        <v>254</v>
+      </c>
+      <c r="E87" t="s">
+        <v>34</v>
+      </c>
+      <c r="G87">
+        <v>1</v>
+      </c>
+      <c r="H87">
+        <v>2</v>
+      </c>
+      <c r="I87" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B88" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C88" t="s">
         <v>61</v>
       </c>
       <c r="D88" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E88" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="G88">
         <v>1</v>
@@ -2693,21 +2690,21 @@
         <v>235</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B89" t="s">
-        <v>58</v>
+        <v>161</v>
       </c>
       <c r="C89" t="s">
         <v>61</v>
       </c>
       <c r="D89" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="E89" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G89">
         <v>1</v>
@@ -2716,6 +2713,58 @@
         <v>2</v>
       </c>
       <c r="I89" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>260</v>
+      </c>
+      <c r="B91" t="s">
+        <v>58</v>
+      </c>
+      <c r="C91" t="s">
+        <v>61</v>
+      </c>
+      <c r="D91" t="s">
+        <v>261</v>
+      </c>
+      <c r="E91" t="s">
+        <v>262</v>
+      </c>
+      <c r="G91">
+        <v>1</v>
+      </c>
+      <c r="H91">
+        <v>2</v>
+      </c>
+      <c r="I91" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>263</v>
+      </c>
+      <c r="B92" t="s">
+        <v>58</v>
+      </c>
+      <c r="C92" t="s">
+        <v>61</v>
+      </c>
+      <c r="D92" t="s">
+        <v>264</v>
+      </c>
+      <c r="E92" t="s">
+        <v>265</v>
+      </c>
+      <c r="G92">
+        <v>1</v>
+      </c>
+      <c r="H92">
+        <v>2</v>
+      </c>
+      <c r="I92" t="s">
         <v>235</v>
       </c>
     </row>
@@ -2732,10 +2781,10 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -2771,13 +2820,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>266</v>
       </c>
@@ -2785,7 +2834,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -2793,7 +2842,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2801,7 +2850,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>76</v>
       </c>
@@ -2809,7 +2858,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>78</v>
       </c>
@@ -2817,7 +2866,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>80</v>
       </c>
@@ -2825,7 +2874,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>82</v>
       </c>
@@ -2833,7 +2882,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>84</v>
       </c>
@@ -2841,7 +2890,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>86</v>
       </c>
@@ -2849,7 +2898,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>88</v>
       </c>
@@ -2857,7 +2906,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -2865,7 +2914,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -2873,7 +2922,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -2881,7 +2930,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>69</v>
       </c>
@@ -2889,7 +2938,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>71</v>
       </c>
@@ -2897,7 +2946,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -2905,7 +2954,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>98</v>
       </c>
@@ -2913,7 +2962,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -2921,7 +2970,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -2929,7 +2978,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>104</v>
       </c>
@@ -2937,7 +2986,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>106</v>
       </c>
@@ -2945,7 +2994,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>108</v>
       </c>
@@ -2953,7 +3002,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>268</v>
       </c>
@@ -2961,7 +3010,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>110</v>
       </c>
@@ -2969,7 +3018,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>112</v>
       </c>
@@ -2977,7 +3026,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>114</v>
       </c>
@@ -2985,7 +3034,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>116</v>
       </c>
@@ -2993,7 +3042,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>118</v>
       </c>
@@ -3001,7 +3050,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>120</v>
       </c>
@@ -3009,7 +3058,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>118</v>
       </c>
@@ -3017,7 +3066,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>123</v>
       </c>
@@ -3025,7 +3074,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>125</v>
       </c>
@@ -3033,7 +3082,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>127</v>
       </c>
@@ -3041,7 +3090,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>129</v>
       </c>
@@ -3049,7 +3098,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>131</v>
       </c>
@@ -3057,7 +3106,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>133</v>
       </c>
@@ -3065,7 +3114,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>135</v>
       </c>
@@ -3073,7 +3122,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>137</v>
       </c>
@@ -3081,12 +3130,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>50</v>
       </c>

</xml_diff>